<commit_message>
Add individual minStock alert
</commit_message>
<xml_diff>
--- a/testExcelFiles/inputFile.xlsx
+++ b/testExcelFiles/inputFile.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10315"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10329"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/ivankikic/Documents/Projects/Croativa/sank-app/testExcelFiles/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{EF7F12A6-98C0-5744-8529-5CE02C312586}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8EB00B69-EE08-974B-AE86-B8C9A9B93BD6}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="1100" yWindow="820" windowWidth="28040" windowHeight="17440" xr2:uid="{E8B426C2-CD1F-6849-8FCB-753DDAEAA3B3}"/>
   </bookViews>
@@ -469,8 +469,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{5071B95D-F9E3-F146-BC12-252727FD21C5}">
   <dimension ref="A1:C25"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="G8" sqref="G8"/>
+    <sheetView tabSelected="1" zoomScale="125" workbookViewId="0">
+      <selection activeCell="B2" sqref="B2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -495,11 +495,11 @@
       </c>
       <c r="B2">
         <f ca="1">RANDBETWEEN(5,30)</f>
-        <v>6</v>
+        <v>21</v>
       </c>
       <c r="C2">
         <f ca="1">RANDBETWEEN(5,30)</f>
-        <v>28</v>
+        <v>24</v>
       </c>
     </row>
     <row r="3" spans="1:3" x14ac:dyDescent="0.2">
@@ -508,11 +508,11 @@
       </c>
       <c r="B3">
         <f t="shared" ref="B3:C25" ca="1" si="0">RANDBETWEEN(5,30)</f>
-        <v>14</v>
+        <v>18</v>
       </c>
       <c r="C3">
         <f t="shared" ca="1" si="0"/>
-        <v>17</v>
+        <v>9</v>
       </c>
     </row>
     <row r="4" spans="1:3" x14ac:dyDescent="0.2">
@@ -521,11 +521,11 @@
       </c>
       <c r="B4">
         <f t="shared" ca="1" si="0"/>
-        <v>6</v>
+        <v>23</v>
       </c>
       <c r="C4">
         <f t="shared" ca="1" si="0"/>
-        <v>12</v>
+        <v>10</v>
       </c>
     </row>
     <row r="5" spans="1:3" x14ac:dyDescent="0.2">
@@ -534,11 +534,11 @@
       </c>
       <c r="B5">
         <f t="shared" ca="1" si="0"/>
-        <v>22</v>
+        <v>29</v>
       </c>
       <c r="C5">
         <f t="shared" ca="1" si="0"/>
-        <v>30</v>
+        <v>11</v>
       </c>
     </row>
     <row r="6" spans="1:3" x14ac:dyDescent="0.2">
@@ -547,11 +547,11 @@
       </c>
       <c r="B6">
         <f t="shared" ca="1" si="0"/>
-        <v>9</v>
+        <v>13</v>
       </c>
       <c r="C6">
         <f t="shared" ca="1" si="0"/>
-        <v>21</v>
+        <v>14</v>
       </c>
     </row>
     <row r="7" spans="1:3" x14ac:dyDescent="0.2">
@@ -560,11 +560,11 @@
       </c>
       <c r="B7">
         <f t="shared" ca="1" si="0"/>
-        <v>27</v>
+        <v>8</v>
       </c>
       <c r="C7">
         <f t="shared" ca="1" si="0"/>
-        <v>29</v>
+        <v>8</v>
       </c>
     </row>
     <row r="8" spans="1:3" x14ac:dyDescent="0.2">
@@ -573,11 +573,11 @@
       </c>
       <c r="B8">
         <f t="shared" ca="1" si="0"/>
-        <v>7</v>
+        <v>11</v>
       </c>
       <c r="C8">
         <f t="shared" ca="1" si="0"/>
-        <v>7</v>
+        <v>17</v>
       </c>
     </row>
     <row r="9" spans="1:3" x14ac:dyDescent="0.2">
@@ -586,11 +586,11 @@
       </c>
       <c r="B9">
         <f t="shared" ca="1" si="0"/>
-        <v>8</v>
+        <v>27</v>
       </c>
       <c r="C9">
         <f t="shared" ca="1" si="0"/>
-        <v>17</v>
+        <v>7</v>
       </c>
     </row>
     <row r="10" spans="1:3" x14ac:dyDescent="0.2">
@@ -599,11 +599,11 @@
       </c>
       <c r="B10">
         <f t="shared" ca="1" si="0"/>
-        <v>13</v>
+        <v>5</v>
       </c>
       <c r="C10">
         <f t="shared" ca="1" si="0"/>
-        <v>25</v>
+        <v>19</v>
       </c>
     </row>
     <row r="11" spans="1:3" x14ac:dyDescent="0.2">
@@ -612,11 +612,11 @@
       </c>
       <c r="B11">
         <f t="shared" ca="1" si="0"/>
-        <v>12</v>
+        <v>5</v>
       </c>
       <c r="C11">
         <f t="shared" ca="1" si="0"/>
-        <v>5</v>
+        <v>18</v>
       </c>
     </row>
     <row r="12" spans="1:3" x14ac:dyDescent="0.2">
@@ -625,11 +625,11 @@
       </c>
       <c r="B12">
         <f t="shared" ca="1" si="0"/>
-        <v>19</v>
+        <v>7</v>
       </c>
       <c r="C12">
         <f t="shared" ca="1" si="0"/>
-        <v>12</v>
+        <v>9</v>
       </c>
     </row>
     <row r="13" spans="1:3" x14ac:dyDescent="0.2">
@@ -638,11 +638,11 @@
       </c>
       <c r="B13">
         <f t="shared" ca="1" si="0"/>
-        <v>24</v>
+        <v>5</v>
       </c>
       <c r="C13">
         <f t="shared" ca="1" si="0"/>
-        <v>20</v>
+        <v>16</v>
       </c>
     </row>
     <row r="14" spans="1:3" x14ac:dyDescent="0.2">
@@ -651,11 +651,11 @@
       </c>
       <c r="B14">
         <f t="shared" ca="1" si="0"/>
-        <v>10</v>
+        <v>14</v>
       </c>
       <c r="C14">
         <f t="shared" ca="1" si="0"/>
-        <v>11</v>
+        <v>22</v>
       </c>
     </row>
     <row r="15" spans="1:3" x14ac:dyDescent="0.2">
@@ -664,11 +664,11 @@
       </c>
       <c r="B15">
         <f t="shared" ca="1" si="0"/>
-        <v>28</v>
+        <v>11</v>
       </c>
       <c r="C15">
         <f t="shared" ca="1" si="0"/>
-        <v>18</v>
+        <v>5</v>
       </c>
     </row>
     <row r="16" spans="1:3" x14ac:dyDescent="0.2">
@@ -677,7 +677,7 @@
       </c>
       <c r="B16">
         <f t="shared" ca="1" si="0"/>
-        <v>19</v>
+        <v>14</v>
       </c>
       <c r="C16">
         <f t="shared" ca="1" si="0"/>
@@ -690,11 +690,11 @@
       </c>
       <c r="B17">
         <f t="shared" ca="1" si="0"/>
-        <v>16</v>
+        <v>29</v>
       </c>
       <c r="C17">
         <f t="shared" ca="1" si="0"/>
-        <v>6</v>
+        <v>11</v>
       </c>
     </row>
     <row r="18" spans="1:3" x14ac:dyDescent="0.2">
@@ -703,11 +703,11 @@
       </c>
       <c r="B18">
         <f t="shared" ca="1" si="0"/>
-        <v>10</v>
+        <v>21</v>
       </c>
       <c r="C18">
         <f t="shared" ca="1" si="0"/>
-        <v>19</v>
+        <v>17</v>
       </c>
     </row>
     <row r="19" spans="1:3" x14ac:dyDescent="0.2">
@@ -716,11 +716,11 @@
       </c>
       <c r="B19">
         <f t="shared" ca="1" si="0"/>
-        <v>16</v>
+        <v>18</v>
       </c>
       <c r="C19">
         <f t="shared" ca="1" si="0"/>
-        <v>27</v>
+        <v>5</v>
       </c>
     </row>
     <row r="20" spans="1:3" x14ac:dyDescent="0.2">
@@ -729,11 +729,11 @@
       </c>
       <c r="B20">
         <f t="shared" ca="1" si="0"/>
-        <v>25</v>
+        <v>27</v>
       </c>
       <c r="C20">
         <f t="shared" ca="1" si="0"/>
-        <v>10</v>
+        <v>24</v>
       </c>
     </row>
     <row r="21" spans="1:3" x14ac:dyDescent="0.2">
@@ -742,11 +742,11 @@
       </c>
       <c r="B21">
         <f t="shared" ca="1" si="0"/>
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="C21">
         <f t="shared" ca="1" si="0"/>
-        <v>14</v>
+        <v>18</v>
       </c>
     </row>
     <row r="22" spans="1:3" x14ac:dyDescent="0.2">
@@ -755,11 +755,11 @@
       </c>
       <c r="B22">
         <f t="shared" ca="1" si="0"/>
-        <v>24</v>
+        <v>5</v>
       </c>
       <c r="C22">
         <f t="shared" ca="1" si="0"/>
-        <v>21</v>
+        <v>22</v>
       </c>
     </row>
     <row r="23" spans="1:3" x14ac:dyDescent="0.2">
@@ -768,11 +768,11 @@
       </c>
       <c r="B23">
         <f t="shared" ca="1" si="0"/>
-        <v>27</v>
+        <v>22</v>
       </c>
       <c r="C23">
         <f t="shared" ca="1" si="0"/>
-        <v>11</v>
+        <v>22</v>
       </c>
     </row>
     <row r="24" spans="1:3" x14ac:dyDescent="0.2">
@@ -781,11 +781,11 @@
       </c>
       <c r="B24">
         <f t="shared" ca="1" si="0"/>
-        <v>19</v>
+        <v>14</v>
       </c>
       <c r="C24">
         <f t="shared" ca="1" si="0"/>
-        <v>29</v>
+        <v>27</v>
       </c>
     </row>
     <row r="25" spans="1:3" x14ac:dyDescent="0.2">
@@ -794,11 +794,11 @@
       </c>
       <c r="B25">
         <f t="shared" ca="1" si="0"/>
-        <v>23</v>
+        <v>25</v>
       </c>
       <c r="C25">
         <f t="shared" ca="1" si="0"/>
-        <v>21</v>
+        <v>13</v>
       </c>
     </row>
   </sheetData>

</xml_diff>